<commit_message>
sepelling mistake in IDs
add S in CRS ID
</commit_message>
<xml_diff>
--- a/SRS_sheet_V1.2.xlsx
+++ b/SRS_sheet_V1.2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dina\Desktop\Project Management\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dina\Documents\GitHub\Foodies\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="121">
   <si>
     <t xml:space="preserve">System Requirements </t>
   </si>
@@ -258,9 +258,6 @@
  to create resturants &amp; menus by 
 English or Franko
  "ex English : Bread &amp; Salt BUT Franko: Aish &amp; Malh"</t>
-  </si>
-  <si>
-    <t>Foodie_CRS_001</t>
   </si>
   <si>
     <t>Foodies_SRS_001</t>
@@ -905,8 +902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.35"/>
@@ -938,13 +935,13 @@
     </row>
     <row r="2" spans="1:5" ht="122.4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>51</v>
+        <v>104</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>5</v>
@@ -955,16 +952,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>106</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>28</v>
@@ -972,16 +969,16 @@
     </row>
     <row r="4" spans="1:5" ht="142.80000000000001" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>106</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>28</v>
@@ -989,16 +986,16 @@
     </row>
     <row r="5" spans="1:5" ht="81.599999999999994" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>106</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>28</v>
@@ -1006,16 +1003,16 @@
     </row>
     <row r="6" spans="1:5" ht="142.80000000000001" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>50</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>28</v>
@@ -1023,16 +1020,16 @@
     </row>
     <row r="7" spans="1:5" ht="61.2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>28</v>
@@ -1040,13 +1037,13 @@
     </row>
     <row r="8" spans="1:5" ht="102" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>28</v>
@@ -1054,13 +1051,13 @@
     </row>
     <row r="9" spans="1:5" ht="122.4" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>28</v>
@@ -1068,16 +1065,16 @@
     </row>
     <row r="10" spans="1:5" ht="142.80000000000001" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>28</v>
@@ -1085,13 +1082,13 @@
     </row>
     <row r="11" spans="1:5" ht="102" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>28</v>
@@ -1099,13 +1096,13 @@
     </row>
     <row r="12" spans="1:5" ht="142.80000000000001" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>28</v>
@@ -1113,13 +1110,13 @@
     </row>
     <row r="13" spans="1:5" ht="102" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>28</v>
@@ -1127,13 +1124,13 @@
     </row>
     <row r="14" spans="1:5" ht="102" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>28</v>
@@ -1141,13 +1138,13 @@
     </row>
     <row r="15" spans="1:5" ht="40.799999999999997" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>28</v>
@@ -1155,16 +1152,16 @@
     </row>
     <row r="16" spans="1:5" ht="81.599999999999994" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>28</v>
@@ -1172,16 +1169,16 @@
     </row>
     <row r="17" spans="1:5" ht="142.80000000000001" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>28</v>
@@ -1189,16 +1186,16 @@
     </row>
     <row r="18" spans="1:5" ht="163.19999999999999" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>28</v>
@@ -1206,16 +1203,16 @@
     </row>
     <row r="19" spans="1:5" ht="40.799999999999997" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>28</v>
@@ -1223,13 +1220,13 @@
     </row>
     <row r="20" spans="1:5" ht="81.599999999999994" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>28</v>
@@ -1237,16 +1234,16 @@
     </row>
     <row r="21" spans="1:5" ht="61.2" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>28</v>
@@ -1254,16 +1251,16 @@
     </row>
     <row r="22" spans="1:5" ht="81.599999999999994" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>28</v>
@@ -1271,16 +1268,16 @@
     </row>
     <row r="23" spans="1:5" ht="81.599999999999994" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>28</v>
@@ -1288,16 +1285,16 @@
     </row>
     <row r="24" spans="1:5" ht="81.599999999999994" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>28</v>
@@ -1305,16 +1302,16 @@
     </row>
     <row r="25" spans="1:5" ht="61.2" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>28</v>
@@ -1322,16 +1319,16 @@
     </row>
     <row r="26" spans="1:5" ht="81.599999999999994" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>28</v>
@@ -1339,16 +1336,16 @@
     </row>
     <row r="27" spans="1:5" ht="102" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>28</v>
@@ -1356,16 +1353,16 @@
     </row>
     <row r="28" spans="1:5" ht="142.80000000000001" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>28</v>
@@ -1373,16 +1370,16 @@
     </row>
     <row r="29" spans="1:5" ht="40.799999999999997" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>28</v>
@@ -1390,13 +1387,13 @@
     </row>
     <row r="30" spans="1:5" ht="81.599999999999994" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>28</v>
@@ -1404,13 +1401,13 @@
     </row>
     <row r="31" spans="1:5" ht="40.799999999999997" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>28</v>
@@ -1418,13 +1415,13 @@
     </row>
     <row r="32" spans="1:5" ht="40.799999999999997" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>28</v>
@@ -1432,13 +1429,13 @@
     </row>
     <row r="33" spans="1:5" ht="102" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>28</v>
@@ -1446,13 +1443,13 @@
     </row>
     <row r="34" spans="1:5" ht="183.6" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>28</v>
@@ -1460,13 +1457,13 @@
     </row>
     <row r="35" spans="1:5" ht="102" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>28</v>
@@ -1474,13 +1471,13 @@
     </row>
     <row r="36" spans="1:5" ht="183.6" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>28</v>
@@ -1488,13 +1485,13 @@
     </row>
     <row r="37" spans="1:5" ht="40.799999999999997" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>28</v>
@@ -1502,13 +1499,13 @@
     </row>
     <row r="38" spans="1:5" ht="81.599999999999994" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>28</v>
@@ -1516,13 +1513,13 @@
     </row>
     <row r="39" spans="1:5" ht="81.599999999999994" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>28</v>
@@ -1530,16 +1527,16 @@
     </row>
     <row r="40" spans="1:5" ht="183.6" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>28</v>
@@ -1547,16 +1544,16 @@
     </row>
     <row r="41" spans="1:5" ht="40.799999999999997" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>28</v>
@@ -1564,16 +1561,16 @@
     </row>
     <row r="42" spans="1:5" ht="61.2" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>45</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>28</v>
@@ -1581,16 +1578,16 @@
     </row>
     <row r="43" spans="1:5" ht="61.8" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>28</v>
@@ -1598,13 +1595,13 @@
     </row>
     <row r="44" spans="1:5" ht="41.4" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B44" s="9" t="s">
         <v>47</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>28</v>
@@ -1612,13 +1609,13 @@
     </row>
     <row r="45" spans="1:5" ht="40.799999999999997" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>28</v>
@@ -1626,32 +1623,32 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update on SRS PR sheet
reviewed on SRS from Foodie_SRS_023 to Foodie_SRS_044
and added notes on it on SRS PR sheet
</commit_message>
<xml_diff>
--- a/SRS_sheet_V1.2.xlsx
+++ b/SRS_sheet_V1.2.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hossa\Documents\GitHub\Foodies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mariam\Documents\GitHub\Foodies\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10646" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SR" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="PeerReviewNotes" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="173">
   <si>
     <t xml:space="preserve">System Requirements </t>
   </si>
@@ -169,21 +169,10 @@
  " There is no nearby restaurants from you :( "</t>
   </si>
   <si>
-    <t>User can search restaurant
- name by substring</t>
-  </si>
-  <si>
     <t>After the user create account or
  login the website should list all
  nearby restaurant to the
  customer location</t>
-  </si>
-  <si>
-    <t>Home page should contain search box</t>
-  </si>
-  <si>
-    <t>User can search for any 
-restaurant he want</t>
   </si>
   <si>
     <t>If the user press to any restaurant he can set an order or show the menu and offers of the restaurant only without order</t>
@@ -202,21 +191,8 @@
 </t>
   </si>
   <si>
-    <t>Offers &amp; Promotions Screen 
-should be display all promos and 
-offers for nearby restaurants for 
-the user location after the user
- press on the Offers &amp; Promotions
- Button</t>
-  </si>
-  <si>
     <t>The user can set an order from
  Offers &amp; Promotions Screen</t>
-  </si>
-  <si>
-    <t>The user can show the restaurants 
-menu only from 
-Offers &amp; Promotions Screen</t>
   </si>
   <si>
     <t>The user can search for restaurant 
@@ -594,9 +570,6 @@
     <t>Foodies_PR_025</t>
   </si>
   <si>
-    <t>Foodies_PR_026</t>
-  </si>
-  <si>
     <t>please specify which page you are !</t>
   </si>
   <si>
@@ -612,6 +585,52 @@
   </si>
   <si>
     <t>The Nearby 5 restaurants shall be sorted alphabetical</t>
+  </si>
+  <si>
+    <t>Mariam Nesiem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">language mistake "restaurants should contains" should be "restaurants shall contain" </t>
+  </si>
+  <si>
+    <t>SRS should be Compatible with SIQ_012</t>
+  </si>
+  <si>
+    <t>User can search for restaurant
+ name by substring</t>
+  </si>
+  <si>
+    <t>Home page shall contain search box</t>
+  </si>
+  <si>
+    <t>User can search for any restaurant he want</t>
+  </si>
+  <si>
+    <t>this requirment is dublicated referring to Foodies_SRS_033</t>
+  </si>
+  <si>
+    <t>Offers &amp; Promotions Screen 
+shall be display all promos and 
+offers for nearby restaurants for 
+the user location after the user
+ press on the Offers &amp; Promotions
+ Button</t>
+  </si>
+  <si>
+    <t>The user can show the restaurants 
+menu only from Offers &amp; Promotions Screen</t>
+  </si>
+  <si>
+    <t>SRS should be Compatible with SIQ_015</t>
+  </si>
+  <si>
+    <t>this requirment is dublicated referring to Foodies_SRS_043</t>
+  </si>
+  <si>
+    <t>SRS should be Compatible with SIQ_017</t>
+  </si>
+  <si>
+    <t>this SRS should ddivided to  two SRS</t>
   </si>
 </sst>
 </file>
@@ -746,9 +765,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -758,9 +774,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -768,6 +781,12 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -779,7 +798,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -810,14 +829,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E27" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E27" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A1:E27"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="ID" dataDxfId="6"/>
-    <tableColumn id="2" name="SRS-ID" dataDxfId="5"/>
-    <tableColumn id="3" name="Document Version" dataDxfId="4"/>
-    <tableColumn id="4" name="Notes" dataDxfId="3"/>
-    <tableColumn id="5" name="Reviewer Name" dataDxfId="2"/>
+    <tableColumn id="1" name="ID" dataDxfId="4"/>
+    <tableColumn id="2" name="SRS-ID" dataDxfId="3"/>
+    <tableColumn id="3" name="Document Version" dataDxfId="2"/>
+    <tableColumn id="4" name="Notes" dataDxfId="1"/>
+    <tableColumn id="5" name="Reviewer Name" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1088,753 +1107,753 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="19.75" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.765625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="54.07421875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="35.69140625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="25.53515625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="22.4609375" style="5" customWidth="1"/>
-    <col min="6" max="16384" width="8.84375" style="5"/>
+    <col min="1" max="1" width="30.7109375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="54.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" style="5" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="12" customFormat="1" ht="62.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:5" s="10" customFormat="1" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="118.3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" ht="101.25" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="118.3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" ht="101.25" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="78.900000000000006" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="98.6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" ht="101.25" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="59.15" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="98.6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" ht="81" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="78.900000000000006" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" ht="81" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="138" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" ht="101.25" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="98.6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" ht="101.25" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="118.3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" ht="101.25" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="98.6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" ht="101.25" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="78.900000000000006" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" ht="81" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="39.450000000000003" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="59.15" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>108</v>
-      </c>
       <c r="E16" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="118.3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" ht="101.25" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>108</v>
-      </c>
       <c r="E17" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="118.3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" ht="121.5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="39.450000000000003" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="78.900000000000006" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="39.450000000000003" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="59.15" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="59.15" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="59.15" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="59.15" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="59.15" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="59.15" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:5" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="138" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5" ht="121.5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D28" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="81" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="81" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="101.25" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="101.25" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="121.5" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="60.75" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="60.75" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="121.5" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="61.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D43" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="E28" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="39.450000000000003" x14ac:dyDescent="0.45">
-      <c r="A29" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="78.900000000000006" x14ac:dyDescent="0.45">
-      <c r="A30" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="39.450000000000003" x14ac:dyDescent="0.45">
-      <c r="A31" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="39.450000000000003" x14ac:dyDescent="0.45">
-      <c r="A32" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="78.900000000000006" x14ac:dyDescent="0.45">
-      <c r="A33" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="98.6" x14ac:dyDescent="0.45">
-      <c r="A34" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="98.6" x14ac:dyDescent="0.45">
-      <c r="A35" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="118.3" x14ac:dyDescent="0.45">
-      <c r="A36" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="39.450000000000003" x14ac:dyDescent="0.45">
-      <c r="A37" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="78.900000000000006" x14ac:dyDescent="0.45">
-      <c r="A38" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B38" s="2" t="s">
+      <c r="E43" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B44" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="78.900000000000006" x14ac:dyDescent="0.45">
-      <c r="A39" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B39" s="2" t="s">
+      <c r="C44" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="118.3" x14ac:dyDescent="0.45">
-      <c r="A40" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="39.450000000000003" x14ac:dyDescent="0.45">
-      <c r="A41" s="1" t="s">
+      <c r="C45" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B41" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="39.450000000000003" x14ac:dyDescent="0.45">
-      <c r="A42" s="1" t="s">
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="59.6" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A43" s="1" t="s">
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="39.9" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A44" s="1" t="s">
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B44" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="39.450000000000003" x14ac:dyDescent="0.45">
-      <c r="A45" s="1" t="s">
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A46" s="1" t="s">
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A47" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A48" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A49" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A50" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A51" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1847,345 +1866,465 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="B14" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.15234375" style="13" customWidth="1"/>
-    <col min="2" max="2" width="23.15234375" style="13" customWidth="1"/>
-    <col min="3" max="3" width="28.3046875" style="13" customWidth="1"/>
-    <col min="4" max="4" width="46.53515625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="29.53515625" style="13" customWidth="1"/>
-    <col min="6" max="16384" width="9.23046875" style="13"/>
+    <col min="1" max="1" width="26.140625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="20" style="11" customWidth="1"/>
+    <col min="4" max="4" width="46.5703125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="29.5703125" style="11" customWidth="1"/>
+    <col min="6" max="16384" width="9.28515625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="C1" s="13" t="s">
+      <c r="B2" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E2" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="E1" s="13" t="s">
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A2" s="13" t="s">
+      <c r="B3" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="E3" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="D2" s="13" t="s">
+      <c r="C4" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D4" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E4" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="99.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A3" s="13" t="s">
+      <c r="B5" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="E5" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A4" s="13" t="s">
+      <c r="C6" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B7" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="46.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="99.45" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="B5" s="13" t="s">
+      <c r="C9" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A6" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A7" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="B7" s="13" t="s">
+      <c r="C10" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="B11" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A8" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="B8" s="13" t="s">
+      <c r="C11" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="46.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="B9" s="13" t="s">
+      <c r="C12" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B13" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A10" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="B10" s="13" t="s">
+      <c r="C13" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="B14" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A11" s="13" t="s">
+      <c r="C14" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B15" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="D11" s="13" t="s">
+      <c r="C15" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="E11" s="13" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A12" s="13" t="s">
+      <c r="B16" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="D12" s="13" t="s">
+      <c r="B17" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D17" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="E12" s="13" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A13" s="13" t="s">
+      <c r="E17" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="D13" s="14" t="s">
+      <c r="B18" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D18" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="E13" s="13" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A14" s="13" t="s">
+      <c r="E18" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="B14" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A15" s="13" t="s">
+      <c r="B19" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="B15" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A16" s="13" t="s">
+      <c r="B20" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="B16" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A17" s="13" t="s">
+      <c r="B21" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A18" s="13" t="s">
+      <c r="B22" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A19" s="13" t="s">
+      <c r="B23" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A20" s="13" t="s">
+      <c r="B24" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A21" s="13" t="s">
+      <c r="B26" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A22" s="13" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A23" s="13" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A24" s="13" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A25" s="13" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A26" s="13" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A27" s="13" t="s">
-        <v>160</v>
+      <c r="C27" s="11" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>